<commit_message>
kanban 2 teste 1
</commit_message>
<xml_diff>
--- a/Copie de Kanban Audio 2 - Gabarit.xlsx
+++ b/Copie de Kanban Audio 2 - Gabarit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2269244\Documents\GitHub\TP-Final-Kanban\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A02E4C1E-E5FA-4E63-ABE3-E290B0B7D0BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55D3630-C2B1-4362-9F9C-48E0456079DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="95">
   <si>
     <t>MON PROJET - KANBAN AUDIO</t>
   </si>
@@ -302,13 +302,16 @@
   </si>
   <si>
     <t>vent gazon(faible)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -369,8 +372,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,6 +432,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -546,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -573,6 +589,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -584,7 +601,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,10 +821,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A93" activeCellId="13" sqref="A7:A19 A21:A24 A26:A35 A37:A46 A48:A57 A60 A64 A66 A68:A71 A73 A74 A76 A84:A91 A93:A99"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J140" sqref="J140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -818,12 +836,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2" t="s">
         <v>1</v>
@@ -831,10 +849,10 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="4"/>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -842,10 +860,10 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="4"/>
       <c r="F3" s="6" t="s">
         <v>3</v>
@@ -853,10 +871,10 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="4"/>
       <c r="F4" s="2" t="s">
         <v>4</v>
@@ -901,7 +919,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -919,7 +937,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -937,7 +955,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -955,7 +973,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -973,7 +991,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -991,7 +1009,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1009,7 +1027,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -1027,7 +1045,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1045,7 +1063,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -1063,7 +1081,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -1081,7 +1099,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -1099,7 +1117,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -1117,7 +1135,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -1145,7 +1163,7 @@
       <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -1163,7 +1181,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -1181,7 +1199,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -1199,7 +1217,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -1227,7 +1245,7 @@
       <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -1245,7 +1263,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -1263,7 +1281,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1281,7 +1299,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1299,7 +1317,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -1317,7 +1335,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -1335,7 +1353,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -1353,7 +1371,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -1371,7 +1389,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -1389,7 +1407,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -1417,7 +1435,7 @@
       <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="12" t="s">
@@ -1435,7 +1453,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -1453,7 +1471,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -1471,7 +1489,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -1489,7 +1507,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="12" t="s">
@@ -1507,7 +1525,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B42" s="12" t="s">
@@ -1525,7 +1543,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="12" t="s">
@@ -1543,7 +1561,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="12" t="s">
@@ -1561,7 +1579,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -1579,7 +1597,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B46" s="12" t="s">
@@ -1607,7 +1625,7 @@
       <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="12" t="s">
@@ -1625,7 +1643,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B49" s="12" t="s">
@@ -1643,7 +1661,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B50" s="12" t="s">
@@ -1661,7 +1679,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="12" t="s">
@@ -1679,7 +1697,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="12" t="s">
@@ -1697,7 +1715,7 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B53" s="12" t="s">
@@ -1715,7 +1733,7 @@
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B54" s="12" t="s">
@@ -1733,7 +1751,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B55" s="12" t="s">
@@ -1751,7 +1769,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B56" s="12" t="s">
@@ -1769,7 +1787,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B57" s="12" t="s">
@@ -1815,7 +1833,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B60" s="12" t="s">
@@ -1879,7 +1897,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B64" s="12" t="s">
@@ -1907,7 +1925,7 @@
       <c r="H65" s="18"/>
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B66" s="12" t="s">
@@ -1935,7 +1953,7 @@
       <c r="H67" s="18"/>
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B68" s="12" t="s">
@@ -1953,7 +1971,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B69" s="12" t="s">
@@ -1971,7 +1989,7 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B70" s="12" t="s">
@@ -1989,7 +2007,7 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B71" s="12" t="s">
@@ -2017,7 +2035,7 @@
       <c r="H72" s="18"/>
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B73" s="12" t="s">
@@ -2035,7 +2053,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B74" s="12" t="s">
@@ -2063,7 +2081,7 @@
       <c r="H75" s="18"/>
     </row>
     <row r="76" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B76" s="12" t="s">
@@ -2091,7 +2109,7 @@
       <c r="H77" s="18"/>
     </row>
     <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B78" s="12" t="s">
@@ -2109,7 +2127,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B79" s="12" t="s">
@@ -2127,7 +2145,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B80" s="12" t="s">
@@ -2145,7 +2163,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="12" t="s">
+      <c r="A81" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B81" s="12" t="s">
@@ -2163,7 +2181,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="31" t="s">
         <v>71</v>
       </c>
       <c r="B82" s="12" t="s">
@@ -2191,7 +2209,7 @@
       <c r="H83" s="18"/>
     </row>
     <row r="84" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="29" t="s">
+      <c r="A84" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -2209,7 +2227,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="29" t="s">
+      <c r="A85" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B85" s="12" t="s">
@@ -2227,7 +2245,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="29" t="s">
+      <c r="A86" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B86" s="12" t="s">
@@ -2245,7 +2263,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="12" t="s">
@@ -2263,7 +2281,7 @@
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="29" t="s">
+      <c r="A88" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B88" s="12" t="s">
@@ -2281,7 +2299,7 @@
       </c>
     </row>
     <row r="89" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="29" t="s">
+      <c r="A89" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B89" s="12" t="s">
@@ -2299,7 +2317,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="29" t="s">
+      <c r="A90" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B90" s="12" t="s">
@@ -2317,7 +2335,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A91" s="29" t="s">
+      <c r="A91" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B91" s="12" t="s">
@@ -2345,7 +2363,7 @@
       <c r="H92" s="18"/>
     </row>
     <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A93" s="29" t="s">
+      <c r="A93" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B93" s="12" t="s">
@@ -2363,7 +2381,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="12" t="s">
@@ -2381,7 +2399,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A95" s="29" t="s">
+      <c r="A95" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B95" s="12" t="s">
@@ -2399,7 +2417,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A96" s="29" t="s">
+      <c r="A96" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B96" s="12" t="s">
@@ -2417,7 +2435,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="29" t="s">
+      <c r="A97" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B97" s="12" t="s">
@@ -2435,7 +2453,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="29" t="s">
+      <c r="A98" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B98" s="12" t="s">
@@ -2453,7 +2471,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="29" t="s">
+      <c r="A99" s="20" t="s">
         <v>13</v>
       </c>
       <c r="B99" s="12" t="s">
@@ -2480,15 +2498,741 @@
       <c r="G100" s="19"/>
       <c r="H100" s="18"/>
     </row>
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D103" s="30"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C111" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D111" s="12"/>
+      <c r="E111" s="12"/>
+      <c r="F111" s="3"/>
+      <c r="G111" s="3"/>
+      <c r="H111" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B112" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C112" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D112" s="12"/>
+      <c r="E112" s="12"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C113" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D113" s="12"/>
+      <c r="E113" s="12"/>
+      <c r="F113" s="3"/>
+      <c r="G113" s="3"/>
+      <c r="H113" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="3"/>
+      <c r="G114" s="3"/>
+      <c r="H114" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D115" s="12"/>
+      <c r="E115" s="12"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="3"/>
+      <c r="H115" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D116" s="12"/>
+      <c r="E116" s="12"/>
+      <c r="F116" s="3"/>
+      <c r="G116" s="3"/>
+      <c r="H116" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C117" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D117" s="12"/>
+      <c r="E117" s="12"/>
+      <c r="F117" s="3"/>
+      <c r="G117" s="3"/>
+      <c r="H117" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D119" s="16"/>
+      <c r="E119" s="16"/>
+      <c r="F119" s="3"/>
+      <c r="G119" s="3"/>
+      <c r="H119" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D120" s="12"/>
+      <c r="E120" s="12"/>
+      <c r="F120" s="3"/>
+      <c r="G120" s="3"/>
+      <c r="H120" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C121" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D121" s="16"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="3"/>
+      <c r="G121" s="3"/>
+      <c r="H121" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B122" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D122" s="16"/>
+      <c r="E122" s="16"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D123" s="12"/>
+      <c r="E123" s="12"/>
+      <c r="F123" s="3"/>
+      <c r="G123" s="3"/>
+      <c r="H123" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B124" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D124" s="16"/>
+      <c r="E124" s="16"/>
+      <c r="F124" s="3"/>
+      <c r="G124" s="3"/>
+      <c r="H124" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D125" s="12"/>
+      <c r="E125" s="12"/>
+      <c r="F125" s="3"/>
+      <c r="G125" s="3"/>
+      <c r="H125" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="3"/>
+      <c r="G126" s="3"/>
+      <c r="H126" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D127" s="16"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="3"/>
+      <c r="G127" s="3"/>
+      <c r="H127" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B128" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D128" s="16"/>
+      <c r="E128" s="16"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="3"/>
+      <c r="H128" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B129" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C129" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D129" s="16"/>
+      <c r="E129" s="16"/>
+      <c r="F129" s="3"/>
+      <c r="G129" s="3"/>
+      <c r="H129" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C130" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D130" s="16"/>
+      <c r="E130" s="16"/>
+      <c r="F130" s="3"/>
+      <c r="G130" s="3"/>
+      <c r="H130" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C131" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D131" s="16"/>
+      <c r="E131" s="16"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B132" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C132" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D132" s="16"/>
+      <c r="E132" s="16"/>
+      <c r="F132" s="3"/>
+      <c r="G132" s="3"/>
+      <c r="H132" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B133" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C133" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D133" s="16"/>
+      <c r="E133" s="16"/>
+      <c r="F133" s="3"/>
+      <c r="G133" s="3"/>
+      <c r="H133" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B134" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C134" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D134" s="16"/>
+      <c r="E134" s="16"/>
+      <c r="F134" s="3"/>
+      <c r="G134" s="3"/>
+      <c r="H134" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B135" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C135" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D135" s="16"/>
+      <c r="E135" s="16"/>
+      <c r="F135" s="3"/>
+      <c r="G135" s="3"/>
+      <c r="H135" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B136" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C136" s="12">
+        <v>1</v>
+      </c>
+      <c r="D136" s="16"/>
+      <c r="E136" s="16"/>
+      <c r="F136" s="3"/>
+      <c r="G136" s="3"/>
+      <c r="H136" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B137" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C137" s="12">
+        <v>2</v>
+      </c>
+      <c r="D137" s="16"/>
+      <c r="E137" s="16"/>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
+      <c r="H137" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B138" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C138" s="12">
+        <v>3</v>
+      </c>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C139" s="12">
+        <v>4</v>
+      </c>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="3"/>
+      <c r="G139" s="3"/>
+      <c r="H139" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B140" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C140" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D140" s="16"/>
+      <c r="E140" s="16"/>
+      <c r="F140" s="3"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="J140" s="30" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C141" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D141" s="16"/>
+      <c r="E141" s="16"/>
+      <c r="F141" s="3"/>
+      <c r="G141" s="3"/>
+      <c r="H141" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C142" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D142" s="16"/>
+      <c r="E142" s="16"/>
+      <c r="F142" s="3"/>
+      <c r="G142" s="3"/>
+      <c r="H142" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C143" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D143" s="16"/>
+      <c r="E143" s="16"/>
+      <c r="F143" s="3"/>
+      <c r="G143" s="3"/>
+      <c r="H143" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C144" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="3"/>
+      <c r="G144" s="3"/>
+      <c r="H144" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C145" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D145" s="16"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="3"/>
+      <c r="H145" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B146" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C146" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D146" s="16"/>
+      <c r="E146" s="16"/>
+      <c r="F146" s="3"/>
+      <c r="G146" s="3"/>
+      <c r="H146" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B147" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C147" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D147" s="16"/>
+      <c r="E147" s="16"/>
+      <c r="F147" s="3"/>
+      <c r="G147" s="3"/>
+      <c r="H147" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C148" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D148" s="16"/>
+      <c r="E148" s="16"/>
+      <c r="F148" s="3"/>
+      <c r="G148" s="3"/>
+      <c r="H148" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C149" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D149" s="16"/>
+      <c r="E149" s="16"/>
+      <c r="F149" s="3"/>
+      <c r="G149" s="3"/>
+      <c r="H149" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C150" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D150" s="16"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="3"/>
+      <c r="G150" s="3"/>
+      <c r="H150" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D4"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="A7:A100 H7:H100" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H111:H150 H7:H100 A111:A150 A7:A100" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SFX,Ambience,musique,Antoine,Mathis"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:B20 B22:B100" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:B20 B22:B100 B111:B150" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Joueur,Arme Joueur,Chomper,Spitter,Grenadier (boss),Coffre santé,Interupteur,plaque,Porte,grenade,boule crachat,musique,surface,ambience extra"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B21" xr:uid="{00000000-0002-0000-0000-000002000000}">

</xml_diff>

<commit_message>
version final d'Antoine pour le Kanban
</commit_message>
<xml_diff>
--- a/Copie de Kanban Audio 2 - Gabarit.xlsx
+++ b/Copie de Kanban Audio 2 - Gabarit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2269244\Documents\GitHub\TP-Final-Kanban\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432072E3-0F49-4499-8A4B-4A08F4743894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBFE0E3-2895-403E-81FF-C698D9B36781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="162">
   <si>
     <t>MON PROJET - KANBAN AUDIO</t>
   </si>
@@ -314,13 +314,205 @@
   </si>
   <si>
     <t>recoit domage 4</t>
+  </si>
+  <si>
+    <t>Omonatopés exclamation 1 vocale</t>
+  </si>
+  <si>
+    <t>Omonatopés exclamation 2 vocale</t>
+  </si>
+  <si>
+    <t>pas terre 1</t>
+  </si>
+  <si>
+    <t>pas terre 2</t>
+  </si>
+  <si>
+    <t>pas terre 3</t>
+  </si>
+  <si>
+    <t>pas terre 4</t>
+  </si>
+  <si>
+    <t>pas terre 5</t>
+  </si>
+  <si>
+    <t>pas gazon 1</t>
+  </si>
+  <si>
+    <t>pas gazon 2</t>
+  </si>
+  <si>
+    <t>pas gazon 3</t>
+  </si>
+  <si>
+    <t>pas gazon 4</t>
+  </si>
+  <si>
+    <t>pas gazon 5</t>
+  </si>
+  <si>
+    <t>pas gazon 6</t>
+  </si>
+  <si>
+    <t>pas boue 1</t>
+  </si>
+  <si>
+    <t>pas boue 2</t>
+  </si>
+  <si>
+    <t>pas boue 3</t>
+  </si>
+  <si>
+    <t>pas boue 4</t>
+  </si>
+  <si>
+    <t>pas boue 5</t>
+  </si>
+  <si>
+    <t>pas boue 6</t>
+  </si>
+  <si>
+    <t>pas pierre 1</t>
+  </si>
+  <si>
+    <t>pas pierre 2</t>
+  </si>
+  <si>
+    <t>pas pierre 3</t>
+  </si>
+  <si>
+    <t>pas pierre 4</t>
+  </si>
+  <si>
+    <t>pas pierre 5</t>
+  </si>
+  <si>
+    <t>attaque 1</t>
+  </si>
+  <si>
+    <t>attaque 2</t>
+  </si>
+  <si>
+    <t>attaque 3</t>
+  </si>
+  <si>
+    <t>attaque 4</t>
+  </si>
+  <si>
+    <t>bruit de pas 1</t>
+  </si>
+  <si>
+    <t>bruit de pas 2</t>
+  </si>
+  <si>
+    <t>bruit de pas 3</t>
+  </si>
+  <si>
+    <t>bruit de pas 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Omonatopés grognement 3 vocale</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Omonatopés grognement 4 vocale</t>
+  </si>
+  <si>
+    <t>Omonatopés exclamation 3 vocale</t>
+  </si>
+  <si>
+    <t>Omonatopés exclamation 4 vocale</t>
+  </si>
+  <si>
+    <t>bruit de pas 5</t>
+  </si>
+  <si>
+    <t>bruit de pas 6</t>
+  </si>
+  <si>
+    <t>attaque lancé 1</t>
+  </si>
+  <si>
+    <t>attaque lancé 2</t>
+  </si>
+  <si>
+    <t>attaque lancé 3</t>
+  </si>
+  <si>
+    <t>attaque lancé 4</t>
+  </si>
+  <si>
+    <t>attaque lancé 5</t>
+  </si>
+  <si>
+    <t>bruit d'effort lancé 1</t>
+  </si>
+  <si>
+    <t>bruit d'effort lancé 2</t>
+  </si>
+  <si>
+    <t>bruit d'effort lancé 3</t>
+  </si>
+  <si>
+    <t>bruit d'effort lancé 4</t>
+  </si>
+  <si>
+    <t>bruit d'effort lancé 5</t>
+  </si>
+  <si>
+    <t>Bulle d'acide 1</t>
+  </si>
+  <si>
+    <t>Bulle d'acide 2</t>
+  </si>
+  <si>
+    <t>Bulle d'acide 3</t>
+  </si>
+  <si>
+    <t>Bulle d'acide 4</t>
+  </si>
+  <si>
+    <t>Eclabousure acide 1</t>
+  </si>
+  <si>
+    <t>Eclabousure acide 2</t>
+  </si>
+  <si>
+    <t>Eclabousure acide 3</t>
+  </si>
+  <si>
+    <t>propulseur 1</t>
+  </si>
+  <si>
+    <t>propulseur 2</t>
+  </si>
+  <si>
+    <t>vent par propulseur 1</t>
+  </si>
+  <si>
+    <t>vent par propulseur 2</t>
+  </si>
+  <si>
+    <t>atterissage vaisseaux 1</t>
+  </si>
+  <si>
+    <t>atterissage vaisseaux 2</t>
+  </si>
+  <si>
+    <t>oiseau 1</t>
+  </si>
+  <si>
+    <t>oiseau 2</t>
+  </si>
+  <si>
+    <t>oiseau 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -380,6 +572,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -831,8 +1028,8 @@
   </sheetPr>
   <dimension ref="A1:Q220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I214" sqref="I214"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3323,22 +3520,14 @@
       </c>
     </row>
     <row r="101" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B101" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C101" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D101" s="12"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A101" s="17"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="18"/>
+      <c r="F101" s="18"/>
+      <c r="G101" s="18"/>
+      <c r="H101" s="17"/>
       <c r="J101" s="17"/>
       <c r="K101" s="18"/>
       <c r="L101" s="18"/>
@@ -3349,22 +3538,14 @@
       <c r="Q101" s="17"/>
     </row>
     <row r="102" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B102" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C102" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D102" s="12"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A102" s="17"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="18"/>
+      <c r="F102" s="18"/>
+      <c r="G102" s="18"/>
+      <c r="H102" s="17"/>
       <c r="J102" s="20" t="s">
         <v>13</v>
       </c>
@@ -3383,22 +3564,14 @@
       </c>
     </row>
     <row r="103" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C103" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D103" s="12"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A103" s="17"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="17"/>
       <c r="J103" s="17"/>
       <c r="K103" s="18"/>
       <c r="L103" s="18"/>
@@ -3409,22 +3582,14 @@
       <c r="Q103" s="17"/>
     </row>
     <row r="104" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B104" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C104" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="D104" s="12"/>
-      <c r="E104" s="12"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A104" s="17"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="18"/>
+      <c r="F104" s="18"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="17"/>
       <c r="J104" s="20" t="s">
         <v>13</v>
       </c>
@@ -3443,22 +3608,14 @@
       </c>
     </row>
     <row r="105" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B105" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C105" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D105" s="12"/>
-      <c r="E105" s="12"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A105" s="17"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="17"/>
       <c r="J105" s="20" t="s">
         <v>13</v>
       </c>
@@ -3484,7 +3641,7 @@
         <v>14</v>
       </c>
       <c r="C106" s="12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -3518,7 +3675,7 @@
         <v>14</v>
       </c>
       <c r="C107" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -3552,7 +3709,7 @@
         <v>14</v>
       </c>
       <c r="C108" s="12" t="s">
-        <v>18</v>
+        <v>95</v>
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
@@ -3578,7 +3735,7 @@
         <v>14</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
@@ -3612,7 +3769,7 @@
         <v>14</v>
       </c>
       <c r="C110" s="12" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -3646,7 +3803,7 @@
         <v>14</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -3672,7 +3829,7 @@
         <v>14</v>
       </c>
       <c r="C112" s="12" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
@@ -3706,7 +3863,7 @@
         <v>14</v>
       </c>
       <c r="C113" s="12" t="s">
-        <v>19</v>
+        <v>103</v>
       </c>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
@@ -3732,7 +3889,7 @@
         <v>14</v>
       </c>
       <c r="C114" s="12" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="D114" s="12"/>
       <c r="E114" s="12"/>
@@ -3766,7 +3923,7 @@
         <v>14</v>
       </c>
       <c r="C115" s="12" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="D115" s="12"/>
       <c r="E115" s="12"/>
@@ -3800,7 +3957,7 @@
         <v>14</v>
       </c>
       <c r="C116" s="12" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="D116" s="12"/>
       <c r="E116" s="12"/>
@@ -3834,7 +3991,7 @@
         <v>14</v>
       </c>
       <c r="C117" s="12" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="D117" s="12"/>
       <c r="E117" s="12"/>
@@ -3868,7 +4025,7 @@
         <v>14</v>
       </c>
       <c r="C118" s="12" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="D118" s="12"/>
       <c r="E118" s="12"/>
@@ -3902,7 +4059,7 @@
         <v>14</v>
       </c>
       <c r="C119" s="12" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="D119" s="12"/>
       <c r="E119" s="12"/>
@@ -3928,7 +4085,7 @@
         <v>14</v>
       </c>
       <c r="C120" s="12" t="s">
-        <v>20</v>
+        <v>110</v>
       </c>
       <c r="D120" s="12"/>
       <c r="E120" s="12"/>
@@ -3962,7 +4119,7 @@
         <v>14</v>
       </c>
       <c r="C121" s="12" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
       <c r="D121" s="12"/>
       <c r="E121" s="12"/>
@@ -3996,7 +4153,7 @@
         <v>14</v>
       </c>
       <c r="C122" s="12" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
@@ -4030,7 +4187,7 @@
         <v>14</v>
       </c>
       <c r="C123" s="12" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D123" s="12"/>
       <c r="E123" s="12"/>
@@ -4064,7 +4221,7 @@
         <v>14</v>
       </c>
       <c r="C124" s="12" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="D124" s="12"/>
       <c r="E124" s="12"/>
@@ -4098,7 +4255,7 @@
         <v>14</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="D125" s="12"/>
       <c r="E125" s="12"/>
@@ -4132,7 +4289,7 @@
         <v>14</v>
       </c>
       <c r="C126" s="12" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D126" s="12"/>
       <c r="E126" s="12"/>
@@ -4166,7 +4323,7 @@
         <v>14</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="D127" s="12"/>
       <c r="E127" s="12"/>
@@ -4200,7 +4357,7 @@
         <v>14</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="D128" s="12"/>
       <c r="E128" s="12"/>
@@ -4226,7 +4383,7 @@
         <v>14</v>
       </c>
       <c r="C129" s="12" t="s">
-        <v>22</v>
+        <v>119</v>
       </c>
       <c r="D129" s="12"/>
       <c r="E129" s="12"/>
@@ -4260,7 +4417,7 @@
         <v>14</v>
       </c>
       <c r="C130" s="12" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
@@ -4294,7 +4451,7 @@
         <v>14</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="D131" s="12"/>
       <c r="E131" s="12"/>
@@ -4328,7 +4485,7 @@
         <v>36</v>
       </c>
       <c r="C132" s="12" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
       <c r="D132" s="12"/>
       <c r="E132" s="12"/>
@@ -4362,7 +4519,7 @@
         <v>36</v>
       </c>
       <c r="C133" s="12" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="D133" s="12"/>
       <c r="E133" s="12"/>
@@ -4396,7 +4553,7 @@
         <v>36</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="D134" s="12"/>
       <c r="E134" s="12"/>
@@ -4430,7 +4587,7 @@
         <v>36</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>37</v>
+        <v>125</v>
       </c>
       <c r="D135" s="12"/>
       <c r="E135" s="12"/>
@@ -4464,7 +4621,7 @@
         <v>36</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="D136" s="15"/>
       <c r="E136" s="15"/>
@@ -4482,7 +4639,7 @@
         <v>36</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>38</v>
+        <v>127</v>
       </c>
       <c r="D137" s="15"/>
       <c r="E137" s="15"/>
@@ -4500,7 +4657,7 @@
         <v>36</v>
       </c>
       <c r="C138" s="14" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="D138" s="15"/>
       <c r="E138" s="15"/>
@@ -4518,7 +4675,7 @@
         <v>36</v>
       </c>
       <c r="C139" s="14" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D139" s="15"/>
       <c r="E139" s="15"/>
@@ -4644,7 +4801,7 @@
         <v>36</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>41</v>
+        <v>130</v>
       </c>
       <c r="D146" s="15"/>
       <c r="E146" s="15"/>
@@ -4662,7 +4819,7 @@
         <v>36</v>
       </c>
       <c r="C147" s="12" t="s">
-        <v>42</v>
+        <v>131</v>
       </c>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
@@ -4680,7 +4837,7 @@
         <v>36</v>
       </c>
       <c r="C148" s="14" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D148" s="15"/>
       <c r="E148" s="15"/>
@@ -4715,8 +4872,8 @@
       <c r="B150" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C150" s="14" t="s">
-        <v>43</v>
+      <c r="C150" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="D150" s="15"/>
       <c r="E150" s="15"/>
@@ -4733,11 +4890,11 @@
       <c r="B151" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C151" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D151" s="12"/>
-      <c r="E151" s="12"/>
+      <c r="C151" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D151" s="15"/>
+      <c r="E151" s="15"/>
       <c r="F151" s="3"/>
       <c r="G151" s="3"/>
       <c r="H151" s="17" t="s">
@@ -4752,7 +4909,7 @@
         <v>36</v>
       </c>
       <c r="C152" s="12" t="s">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="D152" s="15"/>
       <c r="E152" s="15"/>
@@ -4770,7 +4927,7 @@
         <v>36</v>
       </c>
       <c r="C153" s="12" t="s">
-        <v>46</v>
+        <v>133</v>
       </c>
       <c r="D153" s="15"/>
       <c r="E153" s="15"/>
@@ -4785,10 +4942,10 @@
         <v>13</v>
       </c>
       <c r="B154" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C154" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="C154" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="D154" s="15"/>
       <c r="E154" s="15"/>
@@ -4803,10 +4960,10 @@
         <v>13</v>
       </c>
       <c r="B155" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C155" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C155" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="D155" s="15"/>
       <c r="E155" s="15"/>
@@ -4824,7 +4981,7 @@
         <v>47</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>38</v>
+        <v>128</v>
       </c>
       <c r="D156" s="15"/>
       <c r="E156" s="15"/>
@@ -4842,7 +4999,7 @@
         <v>47</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="D157" s="15"/>
       <c r="E157" s="15"/>
@@ -4860,7 +5017,7 @@
         <v>47</v>
       </c>
       <c r="C158" s="14" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="D158" s="15"/>
       <c r="E158" s="15"/>
@@ -4878,7 +5035,7 @@
         <v>47</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>38</v>
+        <v>135</v>
       </c>
       <c r="D159" s="15"/>
       <c r="E159" s="15"/>
@@ -4893,10 +5050,10 @@
         <v>13</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C160" s="14" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="C160" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="D160" s="15"/>
       <c r="E160" s="15"/>
@@ -4911,10 +5068,10 @@
         <v>13</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C161" s="14" t="s">
-        <v>38</v>
+        <v>48</v>
+      </c>
+      <c r="C161" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="D161" s="15"/>
       <c r="E161" s="15"/>
@@ -4932,7 +5089,7 @@
         <v>48</v>
       </c>
       <c r="C162" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D162" s="15"/>
       <c r="E162" s="15"/>
@@ -4950,7 +5107,7 @@
         <v>48</v>
       </c>
       <c r="C163" s="12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D163" s="15"/>
       <c r="E163" s="15"/>
@@ -4968,7 +5125,7 @@
         <v>48</v>
       </c>
       <c r="C164" s="12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D164" s="15"/>
       <c r="E164" s="15"/>
@@ -4986,7 +5143,7 @@
         <v>48</v>
       </c>
       <c r="C165" s="12" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D165" s="15"/>
       <c r="E165" s="15"/>
@@ -5004,7 +5161,7 @@
         <v>48</v>
       </c>
       <c r="C166" s="12" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="D166" s="15"/>
       <c r="E166" s="15"/>
@@ -5022,7 +5179,7 @@
         <v>48</v>
       </c>
       <c r="C167" s="12" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="D167" s="15"/>
       <c r="E167" s="15"/>
@@ -5040,7 +5197,7 @@
         <v>48</v>
       </c>
       <c r="C168" s="12" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="D168" s="15"/>
       <c r="E168" s="15"/>
@@ -5058,7 +5215,7 @@
         <v>48</v>
       </c>
       <c r="C169" s="12" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="D169" s="15"/>
       <c r="E169" s="15"/>
@@ -5076,7 +5233,7 @@
         <v>48</v>
       </c>
       <c r="C170" s="12" t="s">
-        <v>38</v>
+        <v>134</v>
       </c>
       <c r="D170" s="15"/>
       <c r="E170" s="15"/>
@@ -5094,7 +5251,7 @@
         <v>48</v>
       </c>
       <c r="C171" s="12" t="s">
-        <v>38</v>
+        <v>136</v>
       </c>
       <c r="D171" s="15"/>
       <c r="E171" s="15"/>
@@ -5112,7 +5269,7 @@
         <v>48</v>
       </c>
       <c r="C172" s="12" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="D172" s="15"/>
       <c r="E172" s="15"/>
@@ -5130,7 +5287,7 @@
         <v>48</v>
       </c>
       <c r="C173" s="12" t="s">
-        <v>38</v>
+        <v>138</v>
       </c>
       <c r="D173" s="15"/>
       <c r="E173" s="15"/>
@@ -5148,7 +5305,7 @@
         <v>48</v>
       </c>
       <c r="C174" s="12" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="D174" s="15"/>
       <c r="E174" s="15"/>
@@ -5166,7 +5323,7 @@
         <v>48</v>
       </c>
       <c r="C175" s="12" t="s">
-        <v>52</v>
+        <v>140</v>
       </c>
       <c r="D175" s="15"/>
       <c r="E175" s="15"/>
@@ -5184,7 +5341,7 @@
         <v>48</v>
       </c>
       <c r="C176" s="12" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="D176" s="15"/>
       <c r="E176" s="15"/>
@@ -5202,7 +5359,7 @@
         <v>48</v>
       </c>
       <c r="C177" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
       <c r="D177" s="15"/>
       <c r="E177" s="15"/>
@@ -5220,7 +5377,7 @@
         <v>48</v>
       </c>
       <c r="C178" s="12" t="s">
-        <v>52</v>
+        <v>143</v>
       </c>
       <c r="D178" s="15"/>
       <c r="E178" s="15"/>
@@ -5238,7 +5395,7 @@
         <v>48</v>
       </c>
       <c r="C179" s="12" t="s">
-        <v>52</v>
+        <v>144</v>
       </c>
       <c r="D179" s="15"/>
       <c r="E179" s="15"/>
@@ -5256,7 +5413,7 @@
         <v>48</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>53</v>
+        <v>145</v>
       </c>
       <c r="D180" s="15"/>
       <c r="E180" s="15"/>
@@ -5271,10 +5428,10 @@
         <v>13</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C181" s="12" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="C181" s="12">
+        <v>1</v>
       </c>
       <c r="D181" s="15"/>
       <c r="E181" s="15"/>
@@ -5289,10 +5446,10 @@
         <v>13</v>
       </c>
       <c r="B182" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C182" s="12" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="C182" s="12">
+        <v>2</v>
       </c>
       <c r="D182" s="15"/>
       <c r="E182" s="15"/>
@@ -5307,10 +5464,10 @@
         <v>13</v>
       </c>
       <c r="B183" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C183" s="12" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="C183" s="12">
+        <v>3</v>
       </c>
       <c r="D183" s="15"/>
       <c r="E183" s="15"/>
@@ -5325,10 +5482,10 @@
         <v>13</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C184" s="12" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="C184" s="12">
+        <v>4</v>
       </c>
       <c r="D184" s="15"/>
       <c r="E184" s="15"/>
@@ -5339,14 +5496,14 @@
       </c>
     </row>
     <row r="185" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A185" s="20" t="s">
-        <v>13</v>
+      <c r="A185" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C185" s="12">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C185" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="D185" s="15"/>
       <c r="E185" s="15"/>
@@ -5357,14 +5514,14 @@
       </c>
     </row>
     <row r="186" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A186" s="20" t="s">
-        <v>13</v>
+      <c r="A186" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C186" s="12">
-        <v>2</v>
+        <v>71</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="D186" s="15"/>
       <c r="E186" s="15"/>
@@ -5375,14 +5532,14 @@
       </c>
     </row>
     <row r="187" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A187" s="20" t="s">
-        <v>13</v>
+      <c r="A187" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="B187" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C187" s="12">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="C187" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="D187" s="15"/>
       <c r="E187" s="15"/>
@@ -5393,14 +5550,14 @@
       </c>
     </row>
     <row r="188" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="20" t="s">
-        <v>13</v>
+      <c r="A188" s="30" t="s">
+        <v>71</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="C188" s="12">
-        <v>4</v>
+        <v>71</v>
+      </c>
+      <c r="C188" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="D188" s="15"/>
       <c r="E188" s="15"/>
@@ -5411,14 +5568,14 @@
       </c>
     </row>
     <row r="189" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="30" t="s">
-        <v>71</v>
+      <c r="A189" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D189" s="15"/>
       <c r="E189" s="15"/>
@@ -5429,14 +5586,14 @@
       </c>
     </row>
     <row r="190" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="30" t="s">
-        <v>71</v>
+      <c r="A190" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>73</v>
+        <v>146</v>
       </c>
       <c r="D190" s="15"/>
       <c r="E190" s="15"/>
@@ -5447,14 +5604,14 @@
       </c>
     </row>
     <row r="191" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A191" s="30" t="s">
-        <v>71</v>
+      <c r="A191" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C191" s="12" t="s">
-        <v>74</v>
+        <v>147</v>
       </c>
       <c r="D191" s="15"/>
       <c r="E191" s="15"/>
@@ -5465,14 +5622,14 @@
       </c>
     </row>
     <row r="192" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A192" s="30" t="s">
-        <v>71</v>
+      <c r="A192" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C192" s="12" t="s">
-        <v>75</v>
+        <v>148</v>
       </c>
       <c r="D192" s="15"/>
       <c r="E192" s="15"/>
@@ -5490,7 +5647,7 @@
         <v>77</v>
       </c>
       <c r="C193" s="12" t="s">
-        <v>78</v>
+        <v>149</v>
       </c>
       <c r="D193" s="15"/>
       <c r="E193" s="15"/>
@@ -5508,7 +5665,7 @@
         <v>77</v>
       </c>
       <c r="C194" s="12" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="D194" s="15"/>
       <c r="E194" s="15"/>
@@ -5526,7 +5683,7 @@
         <v>77</v>
       </c>
       <c r="C195" s="12" t="s">
-        <v>79</v>
+        <v>151</v>
       </c>
       <c r="D195" s="15"/>
       <c r="E195" s="15"/>
@@ -5544,7 +5701,7 @@
         <v>77</v>
       </c>
       <c r="C196" s="12" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="D196" s="15"/>
       <c r="E196" s="15"/>
@@ -5559,10 +5716,10 @@
         <v>13</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C197" s="12" t="s">
-        <v>79</v>
+        <v>153</v>
       </c>
       <c r="D197" s="15"/>
       <c r="E197" s="15"/>
@@ -5577,10 +5734,10 @@
         <v>13</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C198" s="12" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="D198" s="15"/>
       <c r="E198" s="15"/>
@@ -5595,10 +5752,10 @@
         <v>13</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C199" s="12" t="s">
-        <v>84</v>
+        <v>155</v>
       </c>
       <c r="D199" s="15"/>
       <c r="E199" s="15"/>
@@ -5613,10 +5770,10 @@
         <v>13</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C200" s="12" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
       <c r="D200" s="15"/>
       <c r="E200" s="15"/>
@@ -5634,7 +5791,7 @@
         <v>86</v>
       </c>
       <c r="C201" s="12" t="s">
-        <v>87</v>
+        <v>157</v>
       </c>
       <c r="D201" s="15"/>
       <c r="E201" s="15"/>
@@ -5652,7 +5809,7 @@
         <v>86</v>
       </c>
       <c r="C202" s="12" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="D202" s="15"/>
       <c r="E202" s="15"/>
@@ -5663,14 +5820,14 @@
       </c>
     </row>
     <row r="203" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="20" t="s">
-        <v>13</v>
+      <c r="A203" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="B203" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C203" s="12" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="D203" s="15"/>
       <c r="E203" s="15"/>
@@ -5681,14 +5838,14 @@
       </c>
     </row>
     <row r="204" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A204" s="20" t="s">
-        <v>13</v>
+      <c r="A204" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="B204" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C204" s="12" t="s">
-        <v>88</v>
+        <v>160</v>
       </c>
       <c r="D204" s="15"/>
       <c r="E204" s="15"/>
@@ -5699,14 +5856,14 @@
       </c>
     </row>
     <row r="205" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A205" s="20" t="s">
-        <v>13</v>
+      <c r="A205" s="31" t="s">
+        <v>57</v>
       </c>
       <c r="B205" s="12" t="s">
         <v>86</v>
       </c>
       <c r="C205" s="12" t="s">
-        <v>89</v>
+        <v>161</v>
       </c>
       <c r="D205" s="15"/>
       <c r="E205" s="15"/>
@@ -5717,76 +5874,44 @@
       </c>
     </row>
     <row r="206" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A206" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B206" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C206" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D206" s="15"/>
-      <c r="E206" s="15"/>
-      <c r="F206" s="3"/>
-      <c r="G206" s="3"/>
-      <c r="H206" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A206" s="19"/>
+      <c r="B206" s="19"/>
+      <c r="C206" s="19"/>
+      <c r="D206" s="19"/>
+      <c r="E206" s="19"/>
+      <c r="F206" s="19"/>
+      <c r="G206" s="19"/>
+      <c r="H206" s="19"/>
     </row>
     <row r="207" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A207" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B207" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C207" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D207" s="15"/>
-      <c r="E207" s="15"/>
-      <c r="F207" s="3"/>
-      <c r="G207" s="3"/>
-      <c r="H207" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A207" s="19"/>
+      <c r="B207" s="19"/>
+      <c r="C207" s="19"/>
+      <c r="D207" s="19"/>
+      <c r="E207" s="19"/>
+      <c r="F207" s="19"/>
+      <c r="G207" s="19"/>
+      <c r="H207" s="19"/>
     </row>
     <row r="208" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A208" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B208" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C208" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D208" s="15"/>
-      <c r="E208" s="15"/>
-      <c r="F208" s="3"/>
-      <c r="G208" s="3"/>
-      <c r="H208" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A208" s="19"/>
+      <c r="B208" s="19"/>
+      <c r="C208" s="19"/>
+      <c r="D208" s="19"/>
+      <c r="E208" s="19"/>
+      <c r="F208" s="19"/>
+      <c r="G208" s="19"/>
+      <c r="H208" s="19"/>
     </row>
     <row r="209" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A209" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B209" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C209" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D209" s="15"/>
-      <c r="E209" s="15"/>
-      <c r="F209" s="3"/>
-      <c r="G209" s="3"/>
-      <c r="H209" s="17" t="s">
-        <v>16</v>
-      </c>
+      <c r="A209" s="19"/>
+      <c r="B209" s="19"/>
+      <c r="C209" s="19"/>
+      <c r="D209" s="19"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="19"/>
+      <c r="G209" s="19"/>
+      <c r="H209" s="19"/>
     </row>
     <row r="210" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A210" s="19"/>
@@ -5902,11 +6027,12 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D4"/>
   </mergeCells>
+  <phoneticPr fontId="9" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q43:Q135 J43:J135 A7:A209 H7:H209" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="Q43:Q135 J43:J135 H7:H205 A7:A205" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"SFX,Ambience,musique,Antoine,Mathis"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:B12 K58:K135 K43:K56 B14:B209" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B7:B12 K58:K135 K43:K56 B14:B205" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Joueur,Arme Joueur,Chomper,Spitter,Grenadier (boss),Coffre santé,Interupteur,plaque,Porte,grenade,boule crachat,musique,surface,ambience extra"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K57 B13" xr:uid="{D9ABF81F-9AC8-41DA-90D5-DC9A15228764}">

</xml_diff>